<commit_message>
changed Section to Section_
</commit_message>
<xml_diff>
--- a/PhysicalSample.xlsx
+++ b/PhysicalSample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="180" windowWidth="20385" windowHeight="6750" tabRatio="658" activeTab="3"/>
+    <workbookView xWindow="810" yWindow="180" windowWidth="20385" windowHeight="6750" tabRatio="658" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -3682,7 +3682,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2033" uniqueCount="1485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2033" uniqueCount="1484">
   <si>
     <t>IGSN</t>
   </si>
@@ -7875,9 +7875,6 @@
   </si>
   <si>
     <t>Other information about specimen curation--contact information for curator, previous history of curation</t>
-  </si>
-  <si>
-    <t>Section</t>
   </si>
   <si>
     <t>LocationDescription</t>
@@ -10581,7 +10578,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -10608,7 +10605,7 @@
         <v>184</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="90" x14ac:dyDescent="0.2">
@@ -10616,7 +10613,7 @@
         <v>185</v>
       </c>
       <c r="C4" s="136" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.2">
@@ -10807,7 +10804,7 @@
     </row>
     <row r="20" spans="2:5" ht="24" x14ac:dyDescent="0.2">
       <c r="B20" s="74" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="C20" s="81" t="s">
         <v>471</v>
@@ -10822,7 +10819,7 @@
     <row r="21" spans="2:5" ht="36" x14ac:dyDescent="0.2">
       <c r="B21" s="74"/>
       <c r="C21" s="81" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="D21" s="74" t="s">
         <v>192</v>
@@ -11250,8 +11247,8 @@
   </sheetPr>
   <dimension ref="A1:BF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11285,7 +11282,7 @@
     <col min="27" max="27" width="15.140625" style="26" customWidth="1"/>
     <col min="28" max="28" width="5.140625" style="26" customWidth="1"/>
     <col min="29" max="29" width="4.7109375" style="26" customWidth="1"/>
-    <col min="30" max="30" width="7.5703125" style="26" customWidth="1"/>
+    <col min="30" max="30" width="9.85546875" style="26" customWidth="1"/>
     <col min="31" max="31" width="11.28515625" style="26" customWidth="1"/>
     <col min="32" max="32" width="6.42578125" style="26" customWidth="1"/>
     <col min="33" max="33" width="7.42578125" style="26" customWidth="1"/>
@@ -11373,7 +11370,7 @@
       <c r="AY1" s="13"/>
       <c r="BA1" s="20"/>
       <c r="BB1" s="20" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="BC1" s="20"/>
       <c r="BD1" s="20"/>
@@ -11401,10 +11398,10 @@
         <v>164</v>
       </c>
       <c r="H2" s="102" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="I2" s="102" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="J2" s="151" t="s">
         <v>124</v>
@@ -11467,7 +11464,7 @@
         <v>257</v>
       </c>
       <c r="AD2" s="156" t="s">
-        <v>1355</v>
+        <v>304</v>
       </c>
       <c r="AE2" s="156" t="s">
         <v>258</v>
@@ -11482,7 +11479,7 @@
         <v>261</v>
       </c>
       <c r="AI2" s="157" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="AJ2" s="158" t="s">
         <v>241</v>
@@ -11497,25 +11494,25 @@
         <v>243</v>
       </c>
       <c r="AN2" s="159" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="AO2" s="160" t="s">
+        <v>1358</v>
+      </c>
+      <c r="AP2" s="160" t="s">
+        <v>1459</v>
+      </c>
+      <c r="AQ2" s="31" t="s">
         <v>1359</v>
       </c>
-      <c r="AP2" s="160" t="s">
-        <v>1460</v>
-      </c>
-      <c r="AQ2" s="31" t="s">
+      <c r="AR2" s="16" t="s">
         <v>1360</v>
       </c>
-      <c r="AR2" s="16" t="s">
+      <c r="AS2" s="16" t="s">
         <v>1361</v>
       </c>
-      <c r="AS2" s="16" t="s">
+      <c r="AT2" s="16" t="s">
         <v>1362</v>
-      </c>
-      <c r="AT2" s="16" t="s">
-        <v>1363</v>
       </c>
       <c r="AU2" s="16" t="s">
         <v>158</v>
@@ -11533,10 +11530,10 @@
         <v>162</v>
       </c>
       <c r="AZ2" s="14" t="s">
+        <v>1365</v>
+      </c>
+      <c r="BA2" s="31" t="s">
         <v>1366</v>
-      </c>
-      <c r="BA2" s="31" t="s">
-        <v>1367</v>
       </c>
       <c r="BB2" s="31" t="s">
         <v>117</v>
@@ -11545,7 +11542,7 @@
         <v>173</v>
       </c>
       <c r="BD2" s="31" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="BE2" s="22" t="s">
         <v>354</v>
@@ -11623,8 +11620,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -11640,7 +11637,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A1" s="165" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="B1" s="165"/>
       <c r="C1" s="165"/>
@@ -11653,7 +11650,7 @@
     </row>
     <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="166" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="B2" s="166"/>
       <c r="C2" s="166"/>
@@ -11669,7 +11666,7 @@
         <v>297</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>298</v>
@@ -11700,10 +11697,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="98" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="F4" s="129" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36" x14ac:dyDescent="0.2">
@@ -11723,7 +11720,7 @@
         <v>355</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="84" x14ac:dyDescent="0.2">
@@ -11743,7 +11740,7 @@
         <v>310</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="99" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -11799,7 +11796,7 @@
         <v>359</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="84" x14ac:dyDescent="0.2">
@@ -11822,7 +11819,7 @@
     </row>
     <row r="11" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B11" s="122" t="s">
         <v>302</v>
@@ -11834,13 +11831,13 @@
         <v>300</v>
       </c>
       <c r="E11" s="98" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B12" s="122" t="s">
         <v>301</v>
@@ -11852,7 +11849,7 @@
         <v>300</v>
       </c>
       <c r="E12" s="98" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -11870,10 +11867,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="98" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -11893,7 +11890,7 @@
         <v>472</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="48" x14ac:dyDescent="0.2">
@@ -11910,10 +11907,10 @@
         <v>366</v>
       </c>
       <c r="E15" s="98" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="120" x14ac:dyDescent="0.2">
@@ -11930,10 +11927,10 @@
         <v>300</v>
       </c>
       <c r="E16" s="98" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -11968,10 +11965,10 @@
         <v>366</v>
       </c>
       <c r="E18" s="98" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="36" x14ac:dyDescent="0.2">
@@ -11988,10 +11985,10 @@
         <v>300</v>
       </c>
       <c r="E19" s="98" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -12011,7 +12008,7 @@
         <v>313</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="24" x14ac:dyDescent="0.2">
@@ -12049,7 +12046,7 @@
         <v>314</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.2">
@@ -12089,7 +12086,7 @@
         <v>1354</v>
       </c>
       <c r="F24" s="129" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -12144,7 +12141,7 @@
         <v>356</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="36" x14ac:dyDescent="0.2">
@@ -12164,7 +12161,7 @@
         <v>357</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="108" x14ac:dyDescent="0.2">
@@ -12184,7 +12181,7 @@
         <v>318</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -12244,7 +12241,7 @@
     </row>
     <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="33" t="s">
-        <v>1355</v>
+        <v>304</v>
       </c>
       <c r="B33" s="122" t="s">
         <v>305</v>
@@ -12331,7 +12328,7 @@
     </row>
     <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B38" s="36" t="s">
         <v>302</v>
@@ -12358,10 +12355,10 @@
         <v>1</v>
       </c>
       <c r="E39" s="98" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="84" x14ac:dyDescent="0.2">
@@ -12378,10 +12375,10 @@
         <v>1</v>
       </c>
       <c r="E40" s="98" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="72" x14ac:dyDescent="0.2">
@@ -12398,7 +12395,7 @@
         <v>1</v>
       </c>
       <c r="E41" s="98" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -12422,7 +12419,7 @@
     </row>
     <row r="43" spans="1:6" ht="108" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B43" s="36" t="s">
         <v>302</v>
@@ -12434,15 +12431,15 @@
         <v>300</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>1357</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>1358</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="84" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="B44" s="36" t="s">
         <v>305</v>
@@ -12457,12 +12454,12 @@
         <v>360</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B45" s="36" t="s">
         <v>305</v>
@@ -12480,7 +12477,7 @@
     </row>
     <row r="46" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B46" s="36" t="s">
         <v>302</v>
@@ -12492,13 +12489,13 @@
         <v>300</v>
       </c>
       <c r="E46" s="98" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B47" s="122" t="s">
         <v>302</v>
@@ -12513,12 +12510,12 @@
         <v>326</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="B48" s="122" t="s">
         <v>302</v>
@@ -12533,12 +12530,12 @@
         <v>327</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="B49" s="122" t="s">
         <v>302</v>
@@ -12550,10 +12547,10 @@
         <v>300</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>1364</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>1365</v>
       </c>
       <c r="G49" s="1"/>
     </row>
@@ -12622,7 +12619,7 @@
         <v>329</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -12645,7 +12642,7 @@
     </row>
     <row r="55" spans="1:7" ht="72" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B55" s="122" t="s">
         <v>302</v>
@@ -12663,7 +12660,7 @@
     </row>
     <row r="56" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="B56" s="122" t="s">
         <v>301</v>
@@ -12717,7 +12714,7 @@
     </row>
     <row r="59" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A59" s="31" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B59" s="122" t="s">
         <v>303</v>
@@ -12747,7 +12744,7 @@
         <v>300</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="F60" s="1"/>
     </row>
@@ -12765,10 +12762,10 @@
         <v>300</v>
       </c>
       <c r="E61" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>1368</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>1369</v>
       </c>
     </row>
   </sheetData>
@@ -12900,7 +12897,7 @@
         <v>367</v>
       </c>
       <c r="B8" s="127" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -13024,7 +13021,7 @@
         <v>385</v>
       </c>
       <c r="B27" s="127" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="C27" s="11"/>
     </row>
@@ -13138,7 +13135,7 @@
         <v>396</v>
       </c>
       <c r="B41" s="127" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -13515,7 +13512,7 @@
         <v>463</v>
       </c>
       <c r="B110" s="127" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="16.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -13550,285 +13547,285 @@
     </row>
     <row r="118" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A118" s="130" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B118" s="131" t="s">
         <v>1425</v>
-      </c>
-      <c r="B118" s="131" t="s">
-        <v>1426</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="12" x14ac:dyDescent="0.2">
       <c r="A119" s="132" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B119" s="133" t="s">
         <v>1397</v>
-      </c>
-      <c r="B119" s="133" t="s">
-        <v>1398</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A120" s="132" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B120" s="133" t="s">
         <v>1399</v>
-      </c>
-      <c r="B120" s="133" t="s">
-        <v>1400</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="12" x14ac:dyDescent="0.2">
       <c r="A121" s="132" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B121" s="133" t="s">
         <v>1401</v>
-      </c>
-      <c r="B121" s="133" t="s">
-        <v>1402</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A122" s="132" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B122" s="133" t="s">
         <v>1403</v>
-      </c>
-      <c r="B122" s="133" t="s">
-        <v>1404</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A123" s="132" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B123" s="133" t="s">
         <v>1405</v>
-      </c>
-      <c r="B123" s="133" t="s">
-        <v>1406</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A124" s="132" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B124" s="133" t="s">
         <v>1407</v>
-      </c>
-      <c r="B124" s="133" t="s">
-        <v>1408</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A125" s="132" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B125" s="133" t="s">
         <v>1409</v>
-      </c>
-      <c r="B125" s="133" t="s">
-        <v>1410</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A126" s="132" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B126" s="133" t="s">
         <v>1411</v>
-      </c>
-      <c r="B126" s="133" t="s">
-        <v>1412</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="12" x14ac:dyDescent="0.2">
       <c r="A127" s="132" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B127" s="133" t="s">
         <v>1413</v>
-      </c>
-      <c r="B127" s="133" t="s">
-        <v>1414</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="12" x14ac:dyDescent="0.2">
       <c r="A128" s="132" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B128" s="133" t="s">
         <v>1415</v>
-      </c>
-      <c r="B128" s="133" t="s">
-        <v>1416</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A129" s="132" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B129" s="133" t="s">
         <v>1417</v>
-      </c>
-      <c r="B129" s="133" t="s">
-        <v>1418</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="12" x14ac:dyDescent="0.2">
       <c r="A130" s="132" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B130" s="133" t="s">
         <v>1419</v>
-      </c>
-      <c r="B130" s="133" t="s">
-        <v>1420</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="12" x14ac:dyDescent="0.2">
       <c r="A131" s="132" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B131" s="133" t="s">
         <v>1421</v>
-      </c>
-      <c r="B131" s="133" t="s">
-        <v>1422</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="12" x14ac:dyDescent="0.2">
       <c r="A132" s="132" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B132" s="133" t="s">
         <v>1423</v>
-      </c>
-      <c r="B132" s="133" t="s">
-        <v>1424</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="128" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B135" s="127" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A136" s="114" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="114" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="114" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="114" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="114" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="114" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="114" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="114" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="114" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="114" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="114" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="114" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="114" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="114" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="114" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="114" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="114" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="114" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="114" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="114" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="114" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="114" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="114" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="114" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="114" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="114" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="114" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="114" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="114" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="114" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="114" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
   </sheetData>
@@ -17607,7 +17604,7 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -19684,13 +19681,13 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DF2FC82-BC39-4358-8A56-08290A6D4EDC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>